<commit_message>
Added data to excel
</commit_message>
<xml_diff>
--- a/project2/report/data.xlsx
+++ b/project2/report/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joo Kai\Documents\GitHub\CITS5507-HPC\project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joo Kai\Documents\GitHub\CITS5507-HPC\project2\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C93B41-C8E0-44C4-AC26-CAA509E530F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D28EFB-02EC-4797-AA54-97B773B96BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5100" windowWidth="28110" windowHeight="16440" xr2:uid="{D2A0EE9F-4911-451A-85FB-BDFEE34DEA68}"/>
   </bookViews>
@@ -25,21 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
-  <si>
-    <t>Num threads</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Parallel</t>
-  </si>
-  <si>
-    <t>Seq</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+  <si>
+    <t>SeqBaseT</t>
+  </si>
+  <si>
+    <t>ParBaseT</t>
+  </si>
+  <si>
+    <t>NumFish</t>
+  </si>
+  <si>
+    <t>MPISeqBaseT</t>
+  </si>
+  <si>
+    <t>MPIParBaseT</t>
+  </si>
+  <si>
+    <t>NumThreads</t>
+  </si>
+  <si>
+    <t>NumNodes</t>
   </si>
 </sst>
 </file>
@@ -391,70 +397,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568AB5EE-953A-40D6-91F5-C774C777D341}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10000</v>
+      </c>
+      <c r="B2">
+        <v>3.2684419999999998</v>
+      </c>
+      <c r="C2">
+        <v>3.3780760000000001</v>
+      </c>
+      <c r="D2">
+        <v>0.96280500000000002</v>
+      </c>
+      <c r="E2">
+        <v>1.0972649999999999</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
+      <c r="G2">
+        <v>331.269969</v>
+      </c>
+      <c r="H2">
+        <v>89.734123999999994</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>175.07313300000001</v>
+      </c>
+      <c r="K2">
+        <v>172.31019599999999</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1000000</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100000</v>
+      </c>
+      <c r="B3">
+        <v>32.742747999999999</v>
+      </c>
+      <c r="C3">
+        <v>33.122490999999997</v>
+      </c>
+      <c r="D3">
+        <v>9.0091509999999992</v>
+      </c>
+      <c r="E3">
+        <v>9.1660839999999997</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>327.678245</v>
+      </c>
+      <c r="H3">
+        <v>89.760159999999999</v>
+      </c>
+      <c r="I3">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>1674.065055</v>
+      <c r="J3">
+        <v>116.310136</v>
+      </c>
+      <c r="K3">
+        <v>117.08775799999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>10000000</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1673.794971</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1000000</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>327.678245</v>
+      </c>
+      <c r="C4">
+        <v>330.709878</v>
+      </c>
+      <c r="D4">
+        <v>88.853880000000004</v>
+      </c>
+      <c r="E4">
+        <v>89.760159999999999</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>331.49715800000001</v>
+      </c>
+      <c r="H4">
+        <v>90.355018000000001</v>
+      </c>
+      <c r="I4">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>1668.3133359999999</v>
+      <c r="J4">
+        <v>88.853880000000004</v>
+      </c>
+      <c r="K4">
+        <v>89.760159999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10000000</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
+      <c r="B5">
+        <v>3253.958807</v>
       </c>
       <c r="C5">
-        <v>1667.4859489999999</v>
+        <v>3317.2062340000002</v>
+      </c>
+      <c r="D5">
+        <v>958.066688</v>
+      </c>
+      <c r="E5">
+        <v>965.17265699999996</v>
+      </c>
+      <c r="F5">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>332.09230500000001</v>
+      </c>
+      <c r="H5">
+        <v>90.144876999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added all plots to project 2
</commit_message>
<xml_diff>
--- a/project2/report/data.xlsx
+++ b/project2/report/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joo Kai\Documents\GitHub\CITS5507-HPC\project2\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D28EFB-02EC-4797-AA54-97B773B96BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453EA073-520B-467C-9308-AD4F3E595D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5100" windowWidth="28110" windowHeight="16440" xr2:uid="{D2A0EE9F-4911-451A-85FB-BDFEE34DEA68}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>SeqBaseT</t>
   </si>
@@ -46,6 +46,24 @@
   </si>
   <si>
     <t>NumNodes</t>
+  </si>
+  <si>
+    <t>MPIThreadSafe</t>
+  </si>
+  <si>
+    <t>MPISendRec</t>
+  </si>
+  <si>
+    <t>MPISeq</t>
+  </si>
+  <si>
+    <t>MPIParBaseNodes</t>
+  </si>
+  <si>
+    <t>ParBase</t>
+  </si>
+  <si>
+    <t>MPIParBase</t>
   </si>
 </sst>
 </file>
@@ -397,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568AB5EE-953A-40D6-91F5-C774C777D341}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,10 +431,12 @@
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -436,22 +456,28 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10000</v>
       </c>
@@ -471,22 +497,28 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <v>331.269969</v>
+        <v>331.12</v>
       </c>
       <c r="H2">
         <v>89.734123999999994</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>175.07313300000001</v>
+        <v>327.678245</v>
       </c>
       <c r="K2">
-        <v>172.31019599999999</v>
+        <v>330.709878</v>
+      </c>
+      <c r="L2">
+        <v>330.709878</v>
+      </c>
+      <c r="M2">
+        <v>327.678245</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>100000</v>
       </c>
@@ -506,22 +538,28 @@
         <v>4</v>
       </c>
       <c r="G3">
-        <v>327.678245</v>
+        <v>331.269969</v>
       </c>
       <c r="H3">
         <v>89.760159999999999</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>116.310136</v>
+        <v>175.07313300000001</v>
       </c>
       <c r="K3">
-        <v>117.08775799999999</v>
+        <v>172.31019599999999</v>
+      </c>
+      <c r="L3">
+        <v>172.460532</v>
+      </c>
+      <c r="M3">
+        <v>177.07665700000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1000000</v>
       </c>
@@ -544,19 +582,25 @@
         <v>331.49715800000001</v>
       </c>
       <c r="H4">
-        <v>90.355018000000001</v>
+        <v>90.144876999999994</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J4">
-        <v>88.853880000000004</v>
+        <v>116.310136</v>
       </c>
       <c r="K4">
-        <v>89.760159999999999</v>
+        <v>117.08775799999999</v>
+      </c>
+      <c r="L4">
+        <v>117.18559999999999</v>
+      </c>
+      <c r="M4">
+        <v>119.907118</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10000000</v>
       </c>
@@ -579,7 +623,22 @@
         <v>332.09230500000001</v>
       </c>
       <c r="H5">
-        <v>90.144876999999994</v>
+        <v>90.355018000000001</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>88.853880000000004</v>
+      </c>
+      <c r="K5">
+        <v>89.760159999999999</v>
+      </c>
+      <c r="L5">
+        <v>89.774897999999993</v>
+      </c>
+      <c r="M5">
+        <v>91.457217999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>